<commit_message>
(File) Descriptive statistics for Galaxy J7 Duo updated
</commit_message>
<xml_diff>
--- a/Analysis/GalaxyJ7/curated_data/Descriptive Statistics for Galaxy J7.xlsx
+++ b/Analysis/GalaxyJ7/curated_data/Descriptive Statistics for Galaxy J7.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA998E7A-FA54-44A8-9CBB-50DA78A56D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A109523-42D4-47A0-B528-630E26FAA21F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -72,7 +85,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.000000"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -189,12 +202,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -421,13 +434,13 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6"/>
@@ -442,17 +455,17 @@
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="7"/>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="7"/>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="I2" s="6"/>
@@ -493,7 +506,8 @@
         <v>7</v>
       </c>
       <c r="B4" s="9">
-        <v>8.4469999999999996E-3</v>
+        <f>0.008447*1000</f>
+        <v>8.4469999999999992</v>
       </c>
       <c r="C4" s="3">
         <v>908.44</v>
@@ -502,7 +516,8 @@
         <v>19.5</v>
       </c>
       <c r="E4" s="9">
-        <v>8.8000000000000005E-3</v>
+        <f>0.0088*1000</f>
+        <v>8.8000000000000007</v>
       </c>
       <c r="F4" s="3">
         <v>859.52</v>
@@ -511,7 +526,8 @@
         <v>19.09</v>
       </c>
       <c r="H4" s="9">
-        <v>7.7980000000000002E-3</v>
+        <f>0.007798*1000</f>
+        <v>7.798</v>
       </c>
       <c r="I4" s="3">
         <v>921.48</v>
@@ -525,7 +541,8 @@
         <v>8</v>
       </c>
       <c r="B5" s="9">
-        <v>3.7910000000000001E-3</v>
+        <f>0.003791*1000</f>
+        <v>3.7909999999999999</v>
       </c>
       <c r="C5" s="3">
         <v>792.61</v>
@@ -534,7 +551,8 @@
         <v>3.54</v>
       </c>
       <c r="E5" s="9">
-        <v>5.4019999999999997E-3</v>
+        <f>0.005402*1000</f>
+        <v>5.4019999999999992</v>
       </c>
       <c r="F5" s="3">
         <v>764.36</v>
@@ -543,7 +561,8 @@
         <v>2.21</v>
       </c>
       <c r="H5" s="9">
-        <v>3.2330000000000002E-3</v>
+        <f>0.003233*1000</f>
+        <v>3.2330000000000001</v>
       </c>
       <c r="I5" s="3">
         <v>750.47</v>
@@ -557,7 +576,8 @@
         <v>9</v>
       </c>
       <c r="B6" s="9">
-        <v>1.6789999999999999E-2</v>
+        <f>0.01679*1000</f>
+        <v>16.79</v>
       </c>
       <c r="C6" s="3">
         <v>3260</v>
@@ -566,7 +586,8 @@
         <v>33.67</v>
       </c>
       <c r="E6" s="9">
-        <v>2.3196999999999999E-2</v>
+        <f>0.023197*1000</f>
+        <v>23.196999999999999</v>
       </c>
       <c r="F6" s="3">
         <v>3113</v>
@@ -575,7 +596,8 @@
         <v>24.44</v>
       </c>
       <c r="H6" s="9">
-        <v>1.4612999999999999E-2</v>
+        <f>0.014613*1000</f>
+        <v>14.613</v>
       </c>
       <c r="I6" s="3">
         <v>3091</v>
@@ -589,7 +611,8 @@
         <v>10</v>
       </c>
       <c r="B7" s="9">
-        <v>1.0272999999999999E-2</v>
+        <f>0.010273*1000</f>
+        <v>10.273</v>
       </c>
       <c r="C7" s="3">
         <v>987</v>
@@ -598,7 +621,8 @@
         <v>19.100000000000001</v>
       </c>
       <c r="E7" s="9">
-        <v>1.0926999999999999E-2</v>
+        <f>0.010927*1000</f>
+        <v>10.927</v>
       </c>
       <c r="F7" s="3">
         <v>1004</v>
@@ -607,7 +631,8 @@
         <v>19.22</v>
       </c>
       <c r="H7" s="9">
-        <v>1.04E-2</v>
+        <f>0.0104*1000</f>
+        <v>10.4</v>
       </c>
       <c r="I7" s="3">
         <v>1145</v>
@@ -621,7 +646,8 @@
         <v>11</v>
       </c>
       <c r="B8" s="9">
-        <v>7.7949999999999998E-3</v>
+        <f>0.007795*1000</f>
+        <v>7.7949999999999999</v>
       </c>
       <c r="C8" s="3">
         <v>655</v>
@@ -630,7 +656,8 @@
         <v>18.2</v>
       </c>
       <c r="E8" s="9">
-        <v>7.0299999999999998E-3</v>
+        <f>0.00703*1000</f>
+        <v>7.0299999999999994</v>
       </c>
       <c r="F8" s="3">
         <v>568</v>
@@ -639,7 +666,8 @@
         <v>18.190000000000001</v>
       </c>
       <c r="H8" s="9">
-        <v>6.8060000000000004E-3</v>
+        <f>0.006806*1000</f>
+        <v>6.806</v>
       </c>
       <c r="I8" s="3">
         <v>615</v>
@@ -653,7 +681,8 @@
         <v>12</v>
       </c>
       <c r="B9" s="9">
-        <v>5.4209999999999996E-3</v>
+        <f>0.005421*1000</f>
+        <v>5.4209999999999994</v>
       </c>
       <c r="C9" s="3">
         <v>396</v>
@@ -662,7 +691,8 @@
         <v>17.690000000000001</v>
       </c>
       <c r="E9" s="9">
-        <v>4.9899999999999996E-3</v>
+        <f>0.00499*1000</f>
+        <v>4.9899999999999993</v>
       </c>
       <c r="F9" s="3">
         <v>297</v>
@@ -671,7 +701,8 @@
         <v>17.670000000000002</v>
       </c>
       <c r="H9" s="9">
-        <v>5.6829999999999997E-3</v>
+        <f>0.005683*1000</f>
+        <v>5.6829999999999998</v>
       </c>
       <c r="I9" s="3">
         <v>421</v>
@@ -685,7 +716,8 @@
         <v>13</v>
       </c>
       <c r="B10" s="9">
-        <v>3.96E-3</v>
+        <f>0.00396*1000</f>
+        <v>3.96</v>
       </c>
       <c r="C10" s="3">
         <v>174</v>
@@ -694,7 +726,8 @@
         <v>17.14</v>
       </c>
       <c r="E10" s="9">
-        <v>3.8319999999999999E-3</v>
+        <f>0.003832*1000</f>
+        <v>3.8319999999999999</v>
       </c>
       <c r="F10" s="3">
         <v>87</v>
@@ -703,7 +736,8 @@
         <v>17.170000000000002</v>
       </c>
       <c r="H10" s="9">
-        <v>2.1689999999999999E-3</v>
+        <f>0.002169*1000</f>
+        <v>2.169</v>
       </c>
       <c r="I10" s="3">
         <v>141</v>
@@ -725,7 +759,7 @@
       <c r="J11" s="4"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="6"/>
@@ -740,17 +774,17 @@
     </row>
     <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="7"/>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="5" t="s">
         <v>2</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="7"/>
-      <c r="H13" s="8" t="s">
+      <c r="H13" s="5" t="s">
         <v>3</v>
       </c>
       <c r="I13" s="6"/>
@@ -791,7 +825,8 @@
         <v>7</v>
       </c>
       <c r="B15" s="9">
-        <v>8.1799999999999998E-3</v>
+        <f>0.00818*1000</f>
+        <v>8.18</v>
       </c>
       <c r="C15" s="3">
         <v>990.92</v>
@@ -800,7 +835,8 @@
         <v>17.66</v>
       </c>
       <c r="E15" s="9">
-        <v>8.8950000000000001E-3</v>
+        <f>0.008895*1000</f>
+        <v>8.8949999999999996</v>
       </c>
       <c r="F15" s="3">
         <v>965.24</v>
@@ -809,7 +845,8 @@
         <v>17.68</v>
       </c>
       <c r="H15" s="9">
-        <v>7.9000000000000008E-3</v>
+        <f>0.0079*1000</f>
+        <v>7.9</v>
       </c>
       <c r="I15" s="3">
         <v>1220.72</v>
@@ -823,7 +860,8 @@
         <v>8</v>
       </c>
       <c r="B16" s="9">
-        <v>3.4819999999999999E-3</v>
+        <f>0.003482*1000</f>
+        <v>3.4819999999999998</v>
       </c>
       <c r="C16" s="3">
         <v>834.99</v>
@@ -832,7 +870,8 @@
         <v>0.25</v>
       </c>
       <c r="E16" s="9">
-        <v>4.5149999999999999E-3</v>
+        <f>0.004515*1000</f>
+        <v>4.5149999999999997</v>
       </c>
       <c r="F16" s="3">
         <v>894.87</v>
@@ -841,7 +880,8 @@
         <v>0.24</v>
       </c>
       <c r="H16" s="9">
-        <v>4.5319999999999996E-3</v>
+        <f>0.004532*1000</f>
+        <v>4.5319999999999991</v>
       </c>
       <c r="I16" s="3">
         <v>1110.55</v>
@@ -855,7 +895,8 @@
         <v>9</v>
       </c>
       <c r="B17" s="9">
-        <v>1.5699999999999999E-2</v>
+        <f>0.0157*1000</f>
+        <v>15.7</v>
       </c>
       <c r="C17" s="3">
         <v>3451</v>
@@ -864,7 +905,8 @@
         <v>18.02</v>
       </c>
       <c r="E17" s="9">
-        <v>1.898E-2</v>
+        <f>0.01898*1000</f>
+        <v>18.98</v>
       </c>
       <c r="F17" s="3">
         <v>3420</v>
@@ -873,7 +915,8 @@
         <v>18.02</v>
       </c>
       <c r="H17" s="9">
-        <v>2.1149999999999999E-2</v>
+        <f>0.02115*1000</f>
+        <v>21.15</v>
       </c>
       <c r="I17" s="3">
         <v>4509</v>
@@ -887,7 +930,8 @@
         <v>10</v>
       </c>
       <c r="B18" s="9">
-        <v>1.01E-2</v>
+        <f>0.0101*1000</f>
+        <v>10.1</v>
       </c>
       <c r="C18" s="3">
         <v>1192</v>
@@ -896,7 +940,8 @@
         <v>17.850000000000001</v>
       </c>
       <c r="E18" s="9">
-        <v>1.074E-2</v>
+        <f>0.01074*1000</f>
+        <v>10.74</v>
       </c>
       <c r="F18" s="3">
         <v>1377</v>
@@ -905,7 +950,8 @@
         <v>17.86</v>
       </c>
       <c r="H18" s="9">
-        <v>1.023E-2</v>
+        <f>0.01023*1000</f>
+        <v>10.229999999999999</v>
       </c>
       <c r="I18" s="3">
         <v>1320</v>
@@ -919,7 +965,8 @@
         <v>11</v>
       </c>
       <c r="B19" s="9">
-        <v>7.1199999999999996E-3</v>
+        <f>0.00712*1000</f>
+        <v>7.1199999999999992</v>
       </c>
       <c r="C19" s="3">
         <v>677</v>
@@ -928,7 +975,8 @@
         <v>17.739999999999998</v>
       </c>
       <c r="E19" s="9">
-        <v>7.8100000000000001E-3</v>
+        <f>0.00781*1000</f>
+        <v>7.8100000000000005</v>
       </c>
       <c r="F19" s="3">
         <v>654</v>
@@ -937,7 +985,8 @@
         <v>17.760000000000002</v>
       </c>
       <c r="H19" s="9">
-        <v>6.4000000000000003E-3</v>
+        <f>0.0064*1000</f>
+        <v>6.4</v>
       </c>
       <c r="I19" s="3">
         <v>845</v>
@@ -951,7 +1000,8 @@
         <v>12</v>
       </c>
       <c r="B20" s="9">
-        <v>5.5300000000000002E-3</v>
+        <f>0.00553*1000</f>
+        <v>5.53</v>
       </c>
       <c r="C20" s="3">
         <v>421</v>
@@ -960,7 +1010,8 @@
         <v>17.43</v>
       </c>
       <c r="E20" s="9">
-        <v>5.5700000000000003E-3</v>
+        <f>0.00557*1000</f>
+        <v>5.57</v>
       </c>
       <c r="F20" s="3">
         <v>349</v>
@@ -969,7 +1020,8 @@
         <v>17.45</v>
       </c>
       <c r="H20" s="9">
-        <v>5.1700000000000001E-3</v>
+        <f>0.00517*1000</f>
+        <v>5.17</v>
       </c>
       <c r="I20" s="3">
         <v>509</v>
@@ -983,7 +1035,8 @@
         <v>13</v>
       </c>
       <c r="B21" s="9">
-        <v>4.2500000000000003E-3</v>
+        <f>0.00425*1000</f>
+        <v>4.25</v>
       </c>
       <c r="C21" s="3">
         <v>188</v>
@@ -992,7 +1045,8 @@
         <v>17.260000000000002</v>
       </c>
       <c r="E21" s="9">
-        <v>3.32E-3</v>
+        <f>0.00332*1000</f>
+        <v>3.32</v>
       </c>
       <c r="F21" s="3">
         <v>83</v>
@@ -1001,7 +1055,8 @@
         <v>17.27</v>
       </c>
       <c r="H21" s="9">
-        <v>2.6199999999999999E-3</v>
+        <f>0.00262*1000</f>
+        <v>2.62</v>
       </c>
       <c r="I21" s="3">
         <v>195</v>

</xml_diff>